<commit_message>
-update BNS dan BSIM write range output
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -14,24 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <x:si>
-    <x:t>=S166-S167-S172-S181</x:t>
+    <x:t>=S156+S158</x:t>
   </x:si>
   <x:si>
-    <x:t>=S172</x:t>
+    <x:t>=SUM(S160:S170,S172:S173,S175:S178)</x:t>
   </x:si>
   <x:si>
-    <x:t>=S231+S151-S154</x:t>
+    <x:t>=SUM(S140:S142,S144)</x:t>
   </x:si>
   <x:si>
-    <x:t>=SUM(S148:S150)</x:t>
+    <x:t>=SUM(S111:S112)</x:t>
   </x:si>
   <x:si>
-    <x:t>=S166+S230</x:t>
-  </x:si>
-  <x:si>
-    <x:t>=SUM(S125:S131)</x:t>
+    <x:t>=SUM(S113:S124)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -390,172 +387,175 @@
   <x:sheetData>
     <x:row r="1" spans="1:1">
       <x:c r="A1" s="0" t="n">
-        <x:v>2042.893421821</x:v>
+        <x:v>9881.997642226</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:1">
       <x:c r="A2" s="0" t="n">
-        <x:v>1422.569847297</x:v>
+        <x:v>5121.785773489</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:1">
       <x:c r="A3" s="0" t="n">
-        <x:v>13.718611228</x:v>
+        <x:v>486.501536245</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:1">
       <x:c r="A4" s="0" t="n">
-        <x:v>453.487921958</x:v>
+        <x:v>1326.976521668</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:1">
       <x:c r="A5" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>439.464905052</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:1">
       <x:c r="A6" s="0" t="n">
-        <x:v>25.221366386</x:v>
+        <x:v>387.726088852</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:1">
       <x:c r="A7" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>3.202816476</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:1">
       <x:c r="A8" s="0" t="n">
-        <x:v>127.895674952</x:v>
+        <x:v>18.420114151</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:1">
       <x:c r="A9" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>40.886859158</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:1">
+      <x:c r="A10" s="0" t="n">
+        <x:v>214.049321634</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:1">
       <x:c r="A11" s="0" t="n">
-        <x:v>6940.15409032959</x:v>
+        <x:v>111.166977433</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:1">
       <x:c r="A12" s="0" t="n">
-        <x:v>921.259256821239</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:1">
       <x:c r="A13" s="0" t="n">
-        <x:v>9.74660083755</x:v>
+        <x:v>37.735069586</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:1">
       <x:c r="A14" s="0" t="n">
-        <x:v>911.512655983689</x:v>
+        <x:v>2011.979603638</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:1">
       <x:c r="A15" s="0" t="n">
-        <x:v>2313.98307734465</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:1">
-      <x:c r="A16" s="0" t="n">
-        <x:v>1972.52069122447</x:v>
-      </x:c>
-    </x:row>
+        <x:v>69.828143696</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:1"/>
     <x:row r="17" spans="1:1">
       <x:c r="A17" s="0" t="n">
-        <x:v>341.46238612018</x:v>
+        <x:v>34181.7888272236</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:1">
       <x:c r="A18" s="0" t="n">
-        <x:v>3704.9117561637</x:v>
+        <x:v>14439.2271738949</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:1">
       <x:c r="A19" s="0" t="n">
-        <x:v>1028.942481386</x:v>
+        <x:v>1518.56524748175</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:1">
       <x:c r="A20" s="0" t="n">
-        <x:v>2675.9692747777</x:v>
+        <x:v>12920.6619264131</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:1">
+      <x:c r="A21" s="0" t="n">
+        <x:v>11681.3279125743</x:v>
       </x:c>
     </x:row>
     <x:row r="22" spans="1:1">
       <x:c r="A22" s="0" t="n">
-        <x:v>10.23978303097</x:v>
+        <x:v>11166.6570189352</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:1">
+      <x:c r="A23" s="0" t="n">
+        <x:v>514.6708936391</x:v>
       </x:c>
     </x:row>
     <x:row r="24" spans="1:1">
       <x:c r="A24" s="0" t="n">
-        <x:v>54.7245251073</x:v>
+        <x:v>8061.23374075445</x:v>
       </x:c>
     </x:row>
     <x:row r="25" spans="1:1">
       <x:c r="A25" s="0" t="n">
-        <x:v>2.43182748426</x:v>
+        <x:v>4622.0156449112</x:v>
       </x:c>
     </x:row>
     <x:row r="26" spans="1:1">
       <x:c r="A26" s="0" t="n">
-        <x:v>0.26897921673</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="27" spans="1:1">
-      <x:c r="A27" s="0" t="n">
-        <x:v>31.91954507898</x:v>
-      </x:c>
-    </x:row>
+        <x:v>3439.21809584325</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="27" spans="1:1"/>
     <x:row r="28" spans="1:1">
       <x:c r="A28" s="0" t="n">
-        <x:v>20.10417332733</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="29" spans="1:1">
-      <x:c r="A29" s="0" t="n">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
+        <x:v>3.064477582</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="29" spans="1:1"/>
     <x:row r="30" spans="1:1">
       <x:c r="A30" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>224.81122655362</x:v>
       </x:c>
     </x:row>
     <x:row r="31" spans="1:1">
       <x:c r="A31" s="0" t="n">
-        <x:v>30.45584640594</x:v>
+        <x:v>24.45590430562</x:v>
       </x:c>
     </x:row>
     <x:row r="32" spans="1:1">
       <x:c r="A32" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>13.148025023</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:1">
       <x:c r="A33" s="0" t="n">
-        <x:v>0.00604336884</x:v>
+        <x:v>81.396190671</x:v>
       </x:c>
     </x:row>
     <x:row r="34" spans="1:1">
       <x:c r="A34" s="0" t="n">
-        <x:v>2.85466216281</x:v>
+        <x:v>98.391316977</x:v>
       </x:c>
     </x:row>
     <x:row r="35" spans="1:1">
       <x:c r="A35" s="0" t="n">
-        <x:v>9.15072307577</x:v>
+        <x:v>7.419789577</x:v>
       </x:c>
     </x:row>
     <x:row r="36" spans="1:1">
       <x:c r="A36" s="0" t="n">
-        <x:v>18.44441779852</x:v>
+        <x:v>159.372282774</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:1">
       <x:c r="A37" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>65.510931762</x:v>
       </x:c>
     </x:row>
     <x:row r="38" spans="1:1">
@@ -565,62 +565,67 @@
     </x:row>
     <x:row r="39" spans="1:1">
       <x:c r="A39" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1.224266335</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:1">
       <x:c r="A40" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>10.678277123</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:1">
       <x:c r="A41" s="0" t="n">
-        <x:v>24.26867870136</x:v>
+        <x:v>20.895840787</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="42" spans="1:1">
+      <x:c r="A42" s="0" t="n">
+        <x:v>29.920058468</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:1">
       <x:c r="A43" s="0" t="n">
-        <x:v>7.00192349621</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="44" spans="1:1">
       <x:c r="A44" s="0" t="n">
-        <x:v>1.619</x:v>
+        <x:v>2.792489049</x:v>
       </x:c>
     </x:row>
     <x:row r="45" spans="1:1">
       <x:c r="A45" s="0" t="n">
-        <x:v>0.00185860147</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="46" spans="1:1">
       <x:c r="A46" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>159.372282774</x:v>
       </x:c>
     </x:row>
     <x:row r="47" spans="1:1">
       <x:c r="A47" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>159.30029479162</x:v>
       </x:c>
     </x:row>
     <x:row r="48" spans="1:1">
-      <x:c r="A48" s="0" t="n">
+      <x:c r="A48" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="49" spans="1:1">
       <x:c r="A49" s="0" t="n">
-        <x:v>0.27957789758</x:v>
+        <x:v>80.60992526724</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:1">
       <x:c r="A50" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>10.96054811</x:v>
       </x:c>
     </x:row>
     <x:row r="51" spans="1:1">
       <x:c r="A51" s="0" t="n">
-        <x:v>0.20115360112</x:v>
+        <x:v>1.60779027213</x:v>
       </x:c>
     </x:row>
     <x:row r="52" spans="1:1">
@@ -630,57 +635,57 @@
     </x:row>
     <x:row r="53" spans="1:1">
       <x:c r="A53" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1.4328961156</x:v>
       </x:c>
     </x:row>
     <x:row r="54" spans="1:1">
       <x:c r="A54" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1.42750400215</x:v>
       </x:c>
     </x:row>
     <x:row r="55" spans="1:1">
       <x:c r="A55" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>2.88087503345</x:v>
       </x:c>
     </x:row>
     <x:row r="56" spans="1:1">
       <x:c r="A56" s="0" t="n">
-        <x:v>0.16879881015</x:v>
+        <x:v>0.28126343721</x:v>
       </x:c>
     </x:row>
     <x:row r="57" spans="1:1">
       <x:c r="A57" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>5.12215745325</x:v>
       </x:c>
     </x:row>
     <x:row r="58" spans="1:1">
       <x:c r="A58" s="0" t="n">
-        <x:v>1.49931931502</x:v>
+        <x:v>0.66789644947</x:v>
       </x:c>
     </x:row>
     <x:row r="59" spans="1:1">
       <x:c r="A59" s="0" t="n">
-        <x:v>3.07673463445</x:v>
+        <x:v>6.608280397</x:v>
       </x:c>
     </x:row>
     <x:row r="60" spans="1:1">
       <x:c r="A60" s="0" t="n">
-        <x:v>0.15548063642</x:v>
+        <x:v>1.16234625529</x:v>
       </x:c>
     </x:row>
     <x:row r="61" spans="1:1">
       <x:c r="A61" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>0.2825507112</x:v>
       </x:c>
     </x:row>
     <x:row r="62" spans="1:1">
       <x:c r="A62" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>22.49514691043</x:v>
       </x:c>
     </x:row>
     <x:row r="63" spans="1:1">
       <x:c r="A63" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1.34014967515</x:v>
       </x:c>
     </x:row>
     <x:row r="64" spans="1:1">
@@ -688,194 +693,215 @@
         <x:v>0</x:v>
       </x:c>
     </x:row>
+    <x:row r="65" spans="1:1">
+      <x:c r="A65" s="0" t="n">
+        <x:v>8.15546117131</x:v>
+      </x:c>
+    </x:row>
     <x:row r="66" spans="1:1">
       <x:c r="A66" s="0" t="n">
-        <x:v>27.64160019684</x:v>
+        <x:v>4.26687441259</x:v>
       </x:c>
     </x:row>
     <x:row r="67" spans="1:1">
       <x:c r="A67" s="0" t="n">
-        <x:v>14.88092518904</x:v>
+        <x:v>-1.19999885559082E-10</x:v>
       </x:c>
     </x:row>
     <x:row r="68" spans="1:1">
       <x:c r="A68" s="0" t="n">
-        <x:v>1.50700973867</x:v>
+        <x:v>10.91137560517</x:v>
       </x:c>
     </x:row>
     <x:row r="69" spans="1:1">
       <x:c r="A69" s="0" t="n">
-        <x:v>2.4954411198</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="70" spans="1:1">
-      <x:c r="A70" s="0" t="n">
-        <x:v>0.87543130961</x:v>
-      </x:c>
-    </x:row>
+        <x:v>1.00680925596</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="70" spans="1:1"/>
     <x:row r="71" spans="1:1">
       <x:c r="A71" s="0" t="n">
-        <x:v>2.9730754765</x:v>
+        <x:v>236.71429903466</x:v>
       </x:c>
     </x:row>
     <x:row r="72" spans="1:1">
       <x:c r="A72" s="0" t="n">
-        <x:v>1.23270002651</x:v>
+        <x:v>91.457008655</x:v>
       </x:c>
     </x:row>
     <x:row r="73" spans="1:1">
       <x:c r="A73" s="0" t="n">
-        <x:v>0.71869417969</x:v>
+        <x:v>8.39123114678</x:v>
       </x:c>
     </x:row>
     <x:row r="74" spans="1:1">
       <x:c r="A74" s="0" t="n">
-        <x:v>0.195634929</x:v>
+        <x:v>19.71726796838</x:v>
       </x:c>
     </x:row>
     <x:row r="75" spans="1:1">
       <x:c r="A75" s="0" t="n">
-        <x:v>0.05997362</x:v>
+        <x:v>22.66461205332</x:v>
       </x:c>
     </x:row>
     <x:row r="76" spans="1:1">
       <x:c r="A76" s="0" t="n">
-        <x:v>0.04981371863</x:v>
+        <x:v>25.8186022509</x:v>
       </x:c>
     </x:row>
     <x:row r="77" spans="1:1">
       <x:c r="A77" s="0" t="n">
-        <x:v>2.65290088939</x:v>
+        <x:v>4.27244231646</x:v>
       </x:c>
     </x:row>
     <x:row r="78" spans="1:1">
       <x:c r="A78" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>1.26396596975</x:v>
       </x:c>
     </x:row>
     <x:row r="79" spans="1:1">
       <x:c r="A79" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>3.30499569397</x:v>
       </x:c>
     </x:row>
     <x:row r="80" spans="1:1">
       <x:c r="A80" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>0.6816279167</x:v>
       </x:c>
     </x:row>
     <x:row r="81" spans="1:1">
       <x:c r="A81" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>0.36141527955</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="82" spans="1:1">
+      <x:c r="A82" s="0" t="n">
+        <x:v>12.40768015028</x:v>
       </x:c>
     </x:row>
     <x:row r="83" spans="1:1">
       <x:c r="A83" s="0" t="n">
-        <x:v>6.95306440156</x:v>
+        <x:v>12.24758418127</x:v>
       </x:c>
     </x:row>
     <x:row r="84" spans="1:1">
       <x:c r="A84" s="0" t="n">
-        <x:v>10.70993609856</x:v>
+        <x:v>5.09581080749001</x:v>
       </x:c>
     </x:row>
     <x:row r="85" spans="1:1">
       <x:c r="A85" s="0" t="n">
-        <x:v>3.756871697</x:v>
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="86" spans="1:1">
       <x:c r="A86" s="0" t="n">
-        <x:v>-0.342394455019999</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="87" spans="1:1">
-      <x:c r="A87" s="0" t="n">
-        <x:v>10.63291952823</x:v>
-      </x:c>
-    </x:row>
+        <x:v>29.03005464481</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="87" spans="1:1"/>
     <x:row r="88" spans="1:1">
       <x:c r="A88" s="0" t="n">
-        <x:v>10.97531398325</x:v>
+        <x:v>0.0629488165800012</x:v>
       </x:c>
     </x:row>
     <x:row r="89" spans="1:1">
       <x:c r="A89" s="0" t="n">
-        <x:v>10.23978303097</x:v>
+        <x:v>5.19059174158</x:v>
       </x:c>
     </x:row>
     <x:row r="90" spans="1:1">
       <x:c r="A90" s="0" t="n">
-        <x:v>0</x:v>
+        <x:v>5.127642925</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="91" spans="1:1">
+      <x:c r="A91" s="0" t="n">
+        <x:v>-0.1943922597</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="92" spans="1:1">
+      <x:c r="A92" s="0" t="n">
+        <x:v>1.231216652</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="93" spans="1:1">
+      <x:c r="A93" s="0" t="n">
+        <x:v>1.4256089117</x:v>
       </x:c>
     </x:row>
     <x:row r="94" spans="1:1">
       <x:c r="A94" s="0" t="n">
-        <x:v>0.000365681608621506</x:v>
+        <x:v>3.064477582</x:v>
       </x:c>
     </x:row>
     <x:row r="95" spans="1:1">
       <x:c r="A95" s="0" t="n">
-        <x:v>1.50295037898423E-05</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="96" spans="1:1">
-      <x:c r="A96" s="0" t="n">
-        <x:v>8.73562802255431E-05</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="97" spans="1:1">
-      <x:c r="A97" s="0" t="n">
-        <x:v>0.000294358501053217</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="98" spans="1:1">
-      <x:c r="A98" s="0" t="n">
-        <x:v>3.19864073681106E-07</x:v>
-      </x:c>
-    </x:row>
+        <x:v>-9.20015736483037E-10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="96" spans="1:1"/>
+    <x:row r="97" spans="1:1"/>
+    <x:row r="98" spans="1:1"/>
     <x:row r="99" spans="1:1">
       <x:c r="A99" s="0" t="n">
-        <x:v>0.000853912462654511</x:v>
+        <x:v>0.000322833104414501</x:v>
       </x:c>
     </x:row>
     <x:row r="100" spans="1:1">
       <x:c r="A100" s="0" t="n">
-        <x:v>0.000883948363883494</x:v>
+        <x:v>8.47556138297388E-07</x:v>
       </x:c>
     </x:row>
     <x:row r="101" spans="1:1">
       <x:c r="A101" s="0" t="n">
-        <x:v>3.62900200073</x:v>
+        <x:v>4.31292858831854E-06</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="102" spans="1:1">
+      <x:c r="A102" s="0" t="n">
+        <x:v>0.000289082281826097</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="103" spans="1:1">
+      <x:c r="A103" s="0" t="n">
+        <x:v>5.00892815794659E-06</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="104" spans="1:1">
+      <x:c r="A104" s="0" t="n">
+        <x:v>0.000988884719047457</x:v>
       </x:c>
     </x:row>
     <x:row r="105" spans="1:1">
-      <x:c r="A105" s="0" t="s">
-        <x:v>0</x:v>
+      <x:c r="A105" s="0" t="n">
+        <x:v>0.000999355641271177</x:v>
       </x:c>
     </x:row>
     <x:row r="106" spans="1:1">
-      <x:c r="A106" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="107" spans="1:1">
-      <x:c r="A107" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-    </x:row>
+      <x:c r="A106" s="0" t="n">
+        <x:v>3.00152876449998</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="107" spans="1:1"/>
     <x:row r="108" spans="1:1">
       <x:c r="A108" s="0" t="s">
-        <x:v>3</x:v>
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="109" spans="1:1">
       <x:c r="A109" s="0" t="s">
-        <x:v>4</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="110" spans="1:1">
       <x:c r="A110" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="111" spans="1:1">
+      <x:c r="A111" s="0" t="s">
+        <x:v>4</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>